<commit_message>
Fix: AI retry logic, generic fallback templates, LinkedIn embedding, bold keywords
</commit_message>
<xml_diff>
--- a/HR_Contact_List.xlsx
+++ b/HR_Contact_List.xlsx
@@ -17849,7 +17849,7 @@
     <t>zulfiqar.syed@netcore.co.in</t>
   </si>
   <si>
-    <t>mohitkvk455@gmail.com</t>
+    <t>akanksha.puri@sourcefuse.com</t>
   </si>
 </sst>
 </file>
@@ -18170,7 +18170,7 @@
   <dimension ref="A1:E1843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49514,9 +49514,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>